<commit_message>
add questions and multiple windows, implicite & explicite wait, handle web table & excel sheet, js executor and screenshot
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\webcheckmate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\ReactProjects\webcheckmate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F036E03D-B89F-4E63-94FE-A7ACD9FB9E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A230B8A-0537-4510-9014-4B965ABC689C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -458,7 +469,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,5 +567,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>